<commit_message>
Add notebooks, src, templates and update schedule file
</commit_message>
<xml_diff>
--- a/schedule/PDM_Table_Week09.xlsx
+++ b/schedule/PDM_Table_Week09.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NFDFC\OneDrive\Desktop\GoldValue-Predictor\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BC311D-6CC6-4DB9-8668-249F8507E2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47837D98-CB35-4D8A-94FC-BC5AA7B5F83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>